<commit_message>
update script to zero pad zip codes that start with 0 as pandas make them into ints and chops leading zeroes off
</commit_message>
<xml_diff>
--- a/jd_template_v2.xlsx
+++ b/jd_template_v2.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10808"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{E02E8AB7-F9E1-3C44-8257-0CA2EF000581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9475789F-30D0-AA40-9458-C679B0B3BE6C}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{E02E8AB7-F9E1-3C44-8257-0CA2EF000581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A68B683B-EE61-F14D-8E65-A654091C145B}"/>
   <bookViews>
-    <workbookView xWindow="1300" yWindow="500" windowWidth="28800" windowHeight="12220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1300" yWindow="500" windowWidth="28800" windowHeight="12220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Outbound Order Info" sheetId="1" r:id="rId1"/>
@@ -165,20 +165,19 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>Outbound Order Info</t>
+  </si>
+  <si>
+    <t>Consignee Info</t>
+  </si>
+  <si>
+    <t>Product Info</t>
+  </si>
+  <si>
+    <t>Service Product Info</t>
+  </si>
+  <si>
     <t>*Consignee District/County</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Outbound Order Info</t>
-  </si>
-  <si>
-    <t>Consignee Info</t>
-  </si>
-  <si>
-    <t>Product Info</t>
-  </si>
-  <si>
-    <t>Service Product Info</t>
   </si>
 </sst>
 </file>
@@ -685,8 +684,8 @@
   </sheetPr>
   <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView topLeftCell="U1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Z1" sqref="Z1:AC1"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -723,7 +722,7 @@
   <sheetData>
     <row r="1" spans="1:34" s="1" customFormat="1" ht="21">
       <c r="A1" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -737,7 +736,7 @@
       <c r="K1" s="6"/>
       <c r="L1" s="7"/>
       <c r="M1" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N1" s="9"/>
       <c r="O1" s="9"/>
@@ -752,7 +751,7 @@
       <c r="X1" s="9"/>
       <c r="Y1" s="9"/>
       <c r="Z1" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AA1" s="6"/>
       <c r="AB1" s="6"/>
@@ -813,7 +812,7 @@
         <v>33</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="R2" s="3" t="s">
         <v>1</v>
@@ -868,8 +867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:F1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -884,11 +883,11 @@
   <sheetData>
     <row r="1" spans="1:6" ht="21">
       <c r="A1" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D1" s="13"/>
       <c r="E1" s="13"/>

</xml_diff>